<commit_message>
뭘 했는지도 이젠 기억이 안나~~~ user interest added (눈물, 등 4가지 - db update 필요)
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,99 +199,113 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>main_img VARCHAR(50) NOT NULL,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prd_name VARCHAR(50) NOT NULL,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price INT(11) NOT NULL,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿼리문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userinfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE `userinfo` (</t>
+  </si>
+  <si>
     <t>`id` VARCHAR(50) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`passwd` INT(11) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`name` VARCHAR(50) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`email` VARCHAR(50) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`tel` INT(11) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`address` MEDIUMTEXT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`gen` VARCHAR(50) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`birth` INT(11) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`pic` VARCHAR(50) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`petname` VARCHAR(50) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`petage` INT(11) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`petbirth` INT(11) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>`petgen` VARCHAR(50) NULL DEFAULT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>`pettype` VARCHAR(50) NULL DEFAULT NULL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main_img VARCHAR(50) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prd_name VARCHAR(50) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>price INT(11) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATE TABLE userinfo (</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>table name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쿼리문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>database</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userinfo</t>
+  </si>
+  <si>
+    <t>`pettype` VARCHAR(50) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`interest0` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`interest1` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`interest2` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>관심1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`interest3` INT(11) NULL DEFAULT NULL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -299,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +331,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -400,7 +423,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -420,6 +443,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -752,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -770,31 +802,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="6" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="E4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -802,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -810,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -818,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -826,7 +858,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -834,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -842,7 +874,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -850,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -858,7 +890,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -866,7 +898,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -874,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -882,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -890,307 +922,344 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="D17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="D18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6">
-      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="D19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="D20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="D21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="D22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="E23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="6" t="s">
+    <row r="25" spans="2:6" s="7" customFormat="1">
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="C27" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
-      <c r="E22" t="s">
+    <row r="28" spans="2:6">
+      <c r="E28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
-      <c r="D23" s="6" t="s">
+    <row r="29" spans="2:6">
+      <c r="D29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="3:6">
-      <c r="D24" s="6" t="s">
+    <row r="30" spans="2:6">
+      <c r="D30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6">
-      <c r="D25" s="6" t="s">
+      <c r="F30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="D31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="D26" s="6" t="s">
+      <c r="F31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="D32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6">
-      <c r="F27" t="s">
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="F33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="3:6">
-      <c r="E28" t="s">
+    <row r="34" spans="3:6">
+      <c r="E34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="6" t="s">
+    <row r="36" spans="3:6">
+      <c r="C36" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="3:6">
-      <c r="E31" t="s">
+    <row r="37" spans="3:6">
+      <c r="E37" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6">
-      <c r="D32" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6">
-      <c r="D33" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6">
-      <c r="D34" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6">
-      <c r="D35" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6">
-      <c r="D36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6">
-      <c r="D37" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="38" spans="3:6">
       <c r="D38" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="3:6">
+      <c r="D39" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="3:6">
-      <c r="E40" t="s">
-        <v>31</v>
+      <c r="D40" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="D41" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="3:6">
-      <c r="C42" s="6" t="s">
-        <v>39</v>
+      <c r="D42" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="3:6">
-      <c r="E43" t="s">
-        <v>44</v>
+      <c r="D43" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="3:6">
       <c r="D44" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="3:6">
-      <c r="D45" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="F45" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="3:6">
-      <c r="D46" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6">
-      <c r="D47" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
-        <v>34</v>
+      <c r="E46" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="3:6">
-      <c r="D48" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" t="s">
-        <v>35</v>
+      <c r="C48" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="3:6">
-      <c r="D49" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" t="s">
-        <v>36</v>
+      <c r="E49" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="3:6">
       <c r="D50" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="3:6">
+      <c r="D51" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="3:6">
-      <c r="E52" t="s">
-        <v>42</v>
+      <c r="D52" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6">
+      <c r="D53" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="3:6">
-      <c r="C54" s="6" t="s">
-        <v>43</v>
+      <c r="D54" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="3:6">
-      <c r="E55" t="s">
-        <v>45</v>
+      <c r="D55" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="3:6">
       <c r="D56" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F56" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="3:6">
-      <c r="D57" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="F57" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="3:6">
-      <c r="D58" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6">
-      <c r="D59" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" t="s">
-        <v>34</v>
+      <c r="E58" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="3:6">
-      <c r="D60" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" t="s">
-        <v>35</v>
+      <c r="C60" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="3:6">
-      <c r="D61" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F61" t="s">
-        <v>36</v>
+      <c r="E61" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:6">
       <c r="D62" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6">
+      <c r="D63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6">
+      <c r="D64" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6">
+      <c r="D65" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6">
+      <c r="D66" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6">
+      <c r="D67" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6">
+      <c r="D68" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F68" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="3:6">
-      <c r="F63" t="s">
+    <row r="69" spans="4:6">
+      <c r="F69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="3:6">
-      <c r="E64" t="s">
+    <row r="70" spans="4:6">
+      <c r="E70" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
point & coupon page added, database updated (please add coupon & point)
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SE_Project3\SOGONG\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD4D8A-ACB8-4BF8-AB4B-DEC48AAE83FB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="36" windowWidth="18876" windowHeight="7476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="204" yWindow="36" windowWidth="18876" windowHeight="7476"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="109">
   <si>
     <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -321,24 +315,120 @@
   </si>
   <si>
     <t>PRIMARY KEY(idx)</t>
+  </si>
+  <si>
+    <t>point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE `point` (</t>
+  </si>
+  <si>
+    <t>`order_num` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`point` VARCHAR(50) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`date` VARCHAR(50) NULL DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문하는 페이지에서 (insert)입력, 마이페이지에서 id별로 (select)보여주기, 주문취소시 삭제 - 주문페이지 제작시 주분번호를 생성 필요함,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE `coupon` (</t>
+  </si>
+  <si>
+    <t>`coupontype` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`end_date` INT(11) NULL DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>`start_date` INT(11) NULL DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>쿠폰종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유효일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠폰 종류를 번호에 따라 정해두고, 판매자 페이지에서 발급하는 기능 추가하기 ( 판매자 페이지에서 coupon table에 insert)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠폰 종류: 1 (5% 할인) 2 (10% 할인) 3 (30% 할인) 4 (1000원 할인)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -347,7 +437,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -356,7 +446,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -497,7 +587,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -556,7 +646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,27 +678,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,24 +712,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -833,21 +887,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="8.77734375" style="1"/>
-    <col min="3" max="3" width="12.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="8.796875" style="1"/>
+    <col min="3" max="3" width="12.8984375" style="6" customWidth="1"/>
     <col min="4" max="4" width="12" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -864,38 +918,62 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:14">
       <c r="C3" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:14">
       <c r="E4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="D5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="L6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
@@ -903,7 +981,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:14">
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
@@ -911,7 +989,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:14">
       <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
@@ -919,7 +997,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:14">
       <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
@@ -927,7 +1005,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:14">
       <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
@@ -935,7 +1013,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:14">
       <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
@@ -943,7 +1021,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:14">
       <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
@@ -951,7 +1029,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:14">
       <c r="D14" s="6" t="s">
         <v>11</v>
       </c>
@@ -959,7 +1037,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:14">
       <c r="D15" s="6" t="s">
         <v>12</v>
       </c>
@@ -967,7 +1045,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:14">
       <c r="D16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1340,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="4:6">
+    <row r="65" spans="3:6">
       <c r="D65" s="6" t="s">
         <v>23</v>
       </c>
@@ -1270,7 +1348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="4:6">
+    <row r="66" spans="3:6">
       <c r="D66" s="6" t="s">
         <v>24</v>
       </c>
@@ -1278,7 +1356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="4:6">
+    <row r="67" spans="3:6">
       <c r="D67" s="6" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1364,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="4:6">
+    <row r="68" spans="3:6">
       <c r="D68" s="6" t="s">
         <v>26</v>
       </c>
@@ -1294,7 +1372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="4:6">
+    <row r="69" spans="3:6">
       <c r="D69" s="6" t="s">
         <v>27</v>
       </c>
@@ -1302,7 +1380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="4:6">
+    <row r="70" spans="3:6">
       <c r="D70" s="6" t="s">
         <v>28</v>
       </c>
@@ -1310,7 +1388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="4:6">
+    <row r="71" spans="3:6">
       <c r="D71" s="6" t="s">
         <v>29</v>
       </c>
@@ -1318,14 +1396,121 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="4:6">
+    <row r="72" spans="3:6">
       <c r="F72" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="4:6">
+    <row r="73" spans="3:6">
       <c r="E73" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6">
+      <c r="C75" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6">
+      <c r="E76" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6">
+      <c r="D77" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6">
+      <c r="D78" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6">
+      <c r="D79" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6">
+      <c r="D80" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6">
+      <c r="E81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6">
+      <c r="C83" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6">
+      <c r="C85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6">
+      <c r="D86" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6">
+      <c r="D87" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6">
+      <c r="D88" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F88" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6">
+      <c r="D89" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F89" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6">
+      <c r="E90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6">
+      <c r="C91" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6">
+      <c r="C92" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1336,12 +1521,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1349,12 +1534,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>